<commit_message>
Add model to test medication effect in MDD group on RT
</commit_message>
<xml_diff>
--- a/data/erp_N170_MDD_On_vs_Off_Medication.xlsx
+++ b/data/erp_N170_MDD_On_vs_Off_Medication.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D06C88-B071-E94B-B850-D7729D3A2877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4EC168-C639-FF45-BB65-6F339AC62575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17080" yWindow="2100" windowWidth="21060" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:I307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H310" sqref="H310"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>